<commit_message>
update navbar switch mode
</commit_message>
<xml_diff>
--- a/other/work.xlsx
+++ b/other/work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\review activity\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BE3A7-3A3B-4A32-93AC-4C692AB154D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BC90CF-A65F-43A7-962F-5D65BAA29B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9720" yWindow="-16320" windowWidth="38640" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11835" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,10 @@
     <sheet name="05-02-22" sheetId="7" r:id="rId6"/>
     <sheet name="06-02-22" sheetId="8" r:id="rId7"/>
     <sheet name="07-02-22" sheetId="9" r:id="rId8"/>
-    <sheet name="end" sheetId="3" r:id="rId9"/>
+    <sheet name="08-02-22" sheetId="10" r:id="rId9"/>
+    <sheet name="09-02-22" sheetId="11" r:id="rId10"/>
+    <sheet name="Feuil1" sheetId="12" r:id="rId11"/>
+    <sheet name="end" sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
   <si>
     <t>date début</t>
   </si>
@@ -69,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +80,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,19 +114,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,32 +412,34 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
         <v>44594</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="7">
         <f>SUM(start:end!E2)</f>
-        <v>1.0368055555555555</v>
+        <v>1.5527777777777776</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -428,8 +448,870 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD6A169-D08F-438C-B7CE-CCBFCDA5D70B}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639FB22D-F42F-4B5A-B797-1C03D76749B5}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.65625</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2-A2</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4">
+        <f>SUM(C2:C40)</f>
+        <v>0.10624999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3-A3</f>
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C40" si="0">B4-A4</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85775D8C-50C0-4880-AA14-0269081E57E5}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.65625</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2-A2</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4">
+        <f>SUM(C2:C40)</f>
+        <v>0.10624999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3-A3</f>
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C40" si="0">B4-A4</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EAE24E-82CA-44C7-A59B-1EFD1DF95F45}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -440,26 +1322,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD6A169-D08F-438C-B7CE-CCBFCDA5D70B}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEE646F-55C8-455D-9C68-3A30DB6FB981}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="3"/>
-    <col min="4" max="4" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -492,19 +1395,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -606,19 +1509,19 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="A1:XFD1048576"/>
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -906,19 +1809,19 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1202,19 +2105,19 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:E40"/>
+      <selection activeCell="G37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1250,7 +2153,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
-        <f t="shared" ref="C3:C40" si="0">B4-A4</f>
+        <f t="shared" ref="C4:C40" si="0">B4-A4</f>
         <v>0</v>
       </c>
     </row>
@@ -1485,45 +2388,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AF92D7-9EEC-4FA1-98D1-799B101C7D4B}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="4">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.49861111111111112</v>
+      </c>
       <c r="C2" s="4">
         <f>B2-A2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>0.13055555555555554</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="4">
         <f>SUM(C2:C40)</f>
-        <v>0</v>
+        <v>0.21944444444444433</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.98472222222222217</v>
+      </c>
       <c r="C3" s="4">
         <f>B3-A3</f>
-        <v>0</v>
+        <v>8.8888888888888795E-2</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1532,8 +2446,8 @@
         <f t="shared" ref="C4:C40" si="0">B4-A4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -1542,8 +2456,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -1552,8 +2466,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -1562,352 +2476,776 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EAE24E-82CA-44C7-A59B-1EFD1DF95F45}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D6580A-CAC7-4B99-985F-98F696CC6B97}">
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2-A2</f>
+        <v>4.7222222222222276E-2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4">
+        <f>SUM(C2:C40)</f>
+        <v>8.4027777777777757E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3-A3</f>
+        <v>6.2500000000000333E-3</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.77986111111111101</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C40" si="0">B4-A4</f>
+        <v>3.0555555555555447E-2</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>